<commit_message>
Añadir más preguntas de prueba
</commit_message>
<xml_diff>
--- a/app/src/main/assets/preguntas.xlsx
+++ b/app/src/main/assets/preguntas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesus\AndroidStudioProjects\PreguntasApp\app\src\main\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0873DE98-BCAF-44ED-989A-4924CEC73EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDDE231-E701-4893-B13F-A95A0D288587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="225" yWindow="0" windowWidth="24135" windowHeight="18660" xr2:uid="{C18DC762-3502-4C4D-8F36-A27D6CD76578}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Preguntador</t>
   </si>
@@ -48,32 +48,47 @@
     <t>Respuesta</t>
   </si>
   <si>
-    <t>un mecanico</t>
-  </si>
-  <si>
-    <t>otro mecanico</t>
-  </si>
-  <si>
-    <t>una pregunta</t>
-  </si>
-  <si>
-    <t>otra pregunta</t>
-  </si>
-  <si>
-    <t>una respuesta</t>
-  </si>
-  <si>
-    <t>otra respuesta</t>
-  </si>
-  <si>
-    <t>prueba</t>
+    <t>preguntador 1</t>
+  </si>
+  <si>
+    <t>pregunta 1</t>
+  </si>
+  <si>
+    <t>respuesta 1</t>
+  </si>
+  <si>
+    <t>respuesta 2</t>
+  </si>
+  <si>
+    <t>respuesta 3</t>
+  </si>
+  <si>
+    <t>respuesta 4</t>
+  </si>
+  <si>
+    <t>preguntador 2</t>
+  </si>
+  <si>
+    <t>preguntador 3</t>
+  </si>
+  <si>
+    <t>preguntador 4</t>
+  </si>
+  <si>
+    <t>pregunta 2</t>
+  </si>
+  <si>
+    <t>pregunta 3</t>
+  </si>
+  <si>
+    <t>pregunta 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +100,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,7 +134,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,20 +449,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F06AC7-37F4-42FF-990C-95875D85371F}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="A1:C4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="224.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="118" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,38 +473,50 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="G5" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{27F06AC7-37F4-42FF-990C-95875D85371F}">
@@ -491,6 +524,7 @@
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Limpiar memoria al hacer build
</commit_message>
<xml_diff>
--- a/app/src/main/assets/preguntas.xlsx
+++ b/app/src/main/assets/preguntas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesus\AndroidStudioProjects\PreguntasApp\app\src\main\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDDE231-E701-4893-B13F-A95A0D288587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFBC7BE-F999-432C-A832-143BF1E174A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="225" yWindow="0" windowWidth="24135" windowHeight="18660" xr2:uid="{C18DC762-3502-4C4D-8F36-A27D6CD76578}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Preguntador</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>pregunta 4</t>
+  </si>
+  <si>
+    <t>preguntador 5</t>
+  </si>
+  <si>
+    <t>pregunta 5</t>
+  </si>
+  <si>
+    <t>respuesta 5</t>
   </si>
 </sst>
 </file>
@@ -449,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F06AC7-37F4-42FF-990C-95875D85371F}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,6 +527,17 @@
       </c>
       <c r="G5" s="2"/>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{27F06AC7-37F4-42FF-990C-95875D85371F}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C83">

</xml_diff>